<commit_message>
Selenium Season 3 Nov 3rd
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/regression/Adactin Master Test Data.xlsx
+++ b/src/test/resources/testdata/excels/regression/Adactin Master Test Data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\006LiveTechWS\HybridFramework\src\test\resources\testdata\excels\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F4B5DF-7D0E-4576-AF30-C3680354B36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98777DC-DCA8-413D-8D5C-2223CF492667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="1128" windowWidth="21624" windowHeight="11112" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="com.adactin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -155,6 +157,12 @@
   </si>
   <si>
     <t>reyaz009</t>
+  </si>
+  <si>
+    <t>Ravi0111</t>
+  </si>
+  <si>
+    <t>Adactin.com - New User Registration</t>
   </si>
 </sst>
 </file>
@@ -549,14 +557,14 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -602,21 +610,24 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -625,21 +636,24 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -728,7 +742,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{339D628B-76D7-4244-B40A-3F8AEE44D028}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{339D628B-76D7-4244-B40A-3F8AEE44D028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -736,95 +750,241 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748E0F06-B48F-42A5-ADF1-F94162B2926F}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCC54A4-5BCB-4E93-AAB3-258D509A2DC8}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB6C74C-8C2A-4369-BDAC-D83FA3B0184F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{ECC9080F-B95D-45B4-AABD-AFDE5490320F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E46D239-7999-4F6F-8AAB-CFE272BC69B2}">
+  <dimension ref="F1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{E261F8A7-DDDE-496C-A27A-7F30EED07B74}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>